<commit_message>
Updates to labor data. Added original labor sources.
</commit_message>
<xml_diff>
--- a/data/Excel Workbooks/Calvin2011/AllDataWorkbook.xlsx
+++ b/data/Excel Workbooks/Calvin2011/AllDataWorkbook.xlsx
@@ -143,7 +143,7 @@
       <sheetName val="CES models"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="0"/>
       <sheetData sheetId="1">
         <row r="1">
           <cell r="A1" t="str">
@@ -915,7 +915,7 @@
             <v>2.3844029847701655</v>
           </cell>
           <cell r="E25">
-            <v>1.353821572975088</v>
+            <v>1.3538215729750882</v>
           </cell>
           <cell r="F25">
             <v>1.2812809321146301</v>
@@ -979,7 +979,7 @@
             <v>2.6028860393862372</v>
           </cell>
           <cell r="E27">
-            <v>1.3900863005956263</v>
+            <v>1.3900863005956265</v>
           </cell>
           <cell r="F27">
             <v>1.3054289607799849</v>
@@ -1043,7 +1043,7 @@
             <v>2.8157773416941714</v>
           </cell>
           <cell r="E29">
-            <v>1.4253238989609147</v>
+            <v>1.4252423807660537</v>
           </cell>
           <cell r="F29">
             <v>1.3228427818565678</v>
@@ -1075,7 +1075,7 @@
             <v>2.8877482718713834</v>
           </cell>
           <cell r="E30">
-            <v>1.4099386983174644</v>
+            <v>1.4100365201512979</v>
           </cell>
           <cell r="F30">
             <v>1.2950473044541364</v>
@@ -1107,7 +1107,7 @@
             <v>2.9040578894188074</v>
           </cell>
           <cell r="E31">
-            <v>1.3323170731707317</v>
+            <v>1.3320833876787965</v>
           </cell>
           <cell r="F31">
             <v>1.2397355944849513</v>
@@ -1139,7 +1139,7 @@
             <v>2.9249375453026043</v>
           </cell>
           <cell r="E32">
-            <v>1.3317627494456763</v>
+            <v>1.3321431676883613</v>
           </cell>
           <cell r="F32">
             <v>1.2865472356391658</v>
@@ -1171,7 +1171,7 @@
             <v>2.9596752763713856</v>
           </cell>
           <cell r="E33">
-            <v>1.3741821007782271</v>
+            <v>1.3521966436241903</v>
           </cell>
           <cell r="F33">
             <v>1.2807607771542442</v>
@@ -1191,14 +1191,14 @@
         </row>
       </sheetData>
       <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
       <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="7"/>
       <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1221,7 +1221,7 @@
       <sheetName val="CES Models"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="0"/>
       <sheetData sheetId="1">
         <row r="2">
           <cell r="A2">
@@ -2249,14 +2249,14 @@
         </row>
       </sheetData>
       <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
       <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="7"/>
       <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2278,7 +2278,7 @@
       <sheetName val="GDP Comparison"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="0"/>
       <sheetData sheetId="1">
         <row r="2">
           <cell r="A2">
@@ -3306,13 +3306,13 @@
         </row>
       </sheetData>
       <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
       <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="7"/>
       <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="9"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -3377,7 +3377,7 @@
             <v>1.0985107132899505</v>
           </cell>
           <cell r="E3">
-            <v>1.025828510517504</v>
+            <v>1.0178691150298789</v>
           </cell>
           <cell r="F3">
             <v>1.0363780582761455</v>
@@ -3409,7 +3409,7 @@
             <v>1.2403796076615936</v>
           </cell>
           <cell r="E4">
-            <v>1.0376896829396873</v>
+            <v>1.0326830865914762</v>
           </cell>
           <cell r="F4">
             <v>1.0914400675409635</v>
@@ -3441,7 +3441,7 @@
             <v>1.4015155899016787</v>
           </cell>
           <cell r="E5">
-            <v>1.0500601886449963</v>
+            <v>1.0455996349512124</v>
           </cell>
           <cell r="F5">
             <v>1.1763434041212082</v>
@@ -3473,7 +3473,7 @@
             <v>1.5763081892356818</v>
           </cell>
           <cell r="E6">
-            <v>1.0615313936827389</v>
+            <v>1.0567805903326029</v>
           </cell>
           <cell r="F6">
             <v>1.2061438588220461</v>
@@ -3505,7 +3505,7 @@
             <v>1.7664083693248671</v>
           </cell>
           <cell r="E7">
-            <v>1.0727162591170047</v>
+            <v>1.0705089171150399</v>
           </cell>
           <cell r="F7">
             <v>1.2677247831214169</v>
@@ -3537,7 +3537,7 @@
             <v>1.9674541842240472</v>
           </cell>
           <cell r="E8">
-            <v>1.0837513469125288</v>
+            <v>1.0855105334223953</v>
           </cell>
           <cell r="F8">
             <v>1.3787805466297578</v>
@@ -3569,7 +3569,7 @@
             <v>2.1905964336379244</v>
           </cell>
           <cell r="E9">
-            <v>1.0944003938069702</v>
+            <v>1.098663887061381</v>
           </cell>
           <cell r="F9">
             <v>1.4239524902210814</v>
@@ -3601,7 +3601,7 @@
             <v>2.422423120154733</v>
           </cell>
           <cell r="E10">
-            <v>1.1039174170433839</v>
+            <v>1.1142496548803333</v>
           </cell>
           <cell r="F10">
             <v>1.4038376564415576</v>
@@ -3633,7 +3633,7 @@
             <v>2.6766750310816048</v>
           </cell>
           <cell r="E11">
-            <v>1.1276859801371437</v>
+            <v>1.131015892925423</v>
           </cell>
           <cell r="F11">
             <v>1.4703668396482878</v>
@@ -3665,7 +3665,7 @@
             <v>2.951721368537525</v>
           </cell>
           <cell r="E12">
-            <v>1.1205569990209538</v>
+            <v>1.142997759030947</v>
           </cell>
           <cell r="F12">
             <v>1.5285411964292384</v>
@@ -3697,7 +3697,7 @@
             <v>3.2685310368893497</v>
           </cell>
           <cell r="E13">
-            <v>1.1431311323141213</v>
+            <v>1.155848264812064</v>
           </cell>
           <cell r="F13">
             <v>1.6867578122761935</v>
@@ -3729,7 +3729,7 @@
             <v>3.6488637897989209</v>
           </cell>
           <cell r="E14">
-            <v>1.1654086471462513</v>
+            <v>1.168481752026193</v>
           </cell>
           <cell r="F14">
             <v>1.8830237738216187</v>
@@ -3761,7 +3761,7 @@
             <v>4.0734919941852414</v>
           </cell>
           <cell r="E15">
-            <v>1.15629138497367</v>
+            <v>1.1779171478102899</v>
           </cell>
           <cell r="F15">
             <v>2.1124705766406309</v>
@@ -3793,7 +3793,7 @@
             <v>4.547123044576896</v>
           </cell>
           <cell r="E16">
-            <v>1.17821720919724</v>
+            <v>1.1900291761365198</v>
           </cell>
           <cell r="F16">
             <v>2.4021902372308266</v>
@@ -3825,7 +3825,7 @@
             <v>5.0819993231312024</v>
           </cell>
           <cell r="E17">
-            <v>1.2000044028108472</v>
+            <v>1.1992960303175253</v>
           </cell>
           <cell r="F17">
             <v>2.6250158150928318</v>
@@ -3857,7 +3857,7 @@
             <v>5.6910146543848299</v>
           </cell>
           <cell r="E18">
-            <v>1.2062880828655347</v>
+            <v>1.2093135026735413</v>
           </cell>
           <cell r="F18">
             <v>2.8062144990974685</v>
@@ -3889,7 +3889,7 @@
             <v>6.3511651437118717</v>
           </cell>
           <cell r="E19">
-            <v>1.210779484188824</v>
+            <v>1.2065325839291203</v>
           </cell>
           <cell r="F19">
             <v>2.9616345564196394</v>
@@ -3921,7 +3921,7 @@
             <v>7.2033298087056554</v>
           </cell>
           <cell r="E20">
-            <v>1.1946446114165401</v>
+            <v>1.210440022781649</v>
           </cell>
           <cell r="F20">
             <v>3.3442903621128823</v>
@@ -3953,7 +3953,7 @@
             <v>8.1441590255894987</v>
           </cell>
           <cell r="E21">
-            <v>1.2004276970273946</v>
+            <v>1.2143930907361127</v>
           </cell>
           <cell r="F21">
             <v>3.5744785772970471</v>
@@ -3985,7 +3985,7 @@
             <v>9.189646888420107</v>
           </cell>
           <cell r="E22">
-            <v>1.2060851609182306</v>
+            <v>1.2239513102511816</v>
           </cell>
           <cell r="F22">
             <v>3.8145090203943046</v>
@@ -4054,7 +4054,7 @@
             <v>ZA</v>
           </cell>
           <cell r="J2" t="str">
-            <v>Calvin 2011</v>
+            <v>Calvin2011</v>
           </cell>
         </row>
         <row r="3">
@@ -4071,7 +4071,7 @@
             <v>1.0012022581544466</v>
           </cell>
           <cell r="E3">
-            <v>1.0210844828674435</v>
+            <v>1.0431185657854123</v>
           </cell>
           <cell r="F3">
             <v>1.0229231762314899</v>
@@ -4086,7 +4086,7 @@
             <v>ZA</v>
           </cell>
           <cell r="J3" t="str">
-            <v>Calvin 2011</v>
+            <v>Calvin2011</v>
           </cell>
         </row>
         <row r="4">
@@ -4103,7 +4103,7 @@
             <v>1.0019236130471145</v>
           </cell>
           <cell r="E4">
-            <v>1.0596971479482411</v>
+            <v>1.0574888746154401</v>
           </cell>
           <cell r="F4">
             <v>1.0226100561442151</v>
@@ -4118,7 +4118,7 @@
             <v>ZA</v>
           </cell>
           <cell r="J4" t="str">
-            <v>Calvin 2011</v>
+            <v>Calvin2011</v>
           </cell>
         </row>
         <row r="5">
@@ -4135,7 +4135,7 @@
             <v>1.0084332311123501</v>
           </cell>
           <cell r="E5">
-            <v>1.1703636849475125</v>
+            <v>1.1799696229951748</v>
           </cell>
           <cell r="F5">
             <v>1.1102322464387493</v>
@@ -4150,7 +4150,7 @@
             <v>ZA</v>
           </cell>
           <cell r="J5" t="str">
-            <v>Calvin 2011</v>
+            <v>Calvin2011</v>
           </cell>
         </row>
         <row r="6">
@@ -4167,7 +4167,7 @@
             <v>1.0226826038472261</v>
           </cell>
           <cell r="E6">
-            <v>1.2756746171943205</v>
+            <v>1.2732863978279441</v>
           </cell>
           <cell r="F6">
             <v>1.1270287190833779</v>
@@ -4182,7 +4182,7 @@
             <v>ZA</v>
           </cell>
           <cell r="J6" t="str">
-            <v>Calvin 2011</v>
+            <v>Calvin2011</v>
           </cell>
         </row>
         <row r="7">
@@ -4199,7 +4199,7 @@
             <v>1.0435775020908837</v>
           </cell>
           <cell r="E7">
-            <v>1.2422655511589069</v>
+            <v>1.2573109473776538</v>
           </cell>
           <cell r="F7">
             <v>1.1424144339714173</v>
@@ -4214,7 +4214,7 @@
             <v>ZA</v>
           </cell>
           <cell r="J7" t="str">
-            <v>Calvin 2011</v>
+            <v>Calvin2011</v>
           </cell>
         </row>
         <row r="8">
@@ -4231,7 +4231,7 @@
             <v>1.0683196264287707</v>
           </cell>
           <cell r="E8">
-            <v>1.2908777646168526</v>
+            <v>1.2752286086734368</v>
           </cell>
           <cell r="F8">
             <v>1.2324433362558471</v>
@@ -4246,7 +4246,7 @@
             <v>ZA</v>
           </cell>
           <cell r="J8" t="str">
-            <v>Calvin 2011</v>
+            <v>Calvin2011</v>
           </cell>
         </row>
         <row r="9">
@@ -4263,7 +4263,7 @@
             <v>1.0959889880122664</v>
           </cell>
           <cell r="E9">
-            <v>1.2885477134940848</v>
+            <v>1.2903948686660907</v>
           </cell>
           <cell r="F9">
             <v>1.1758332441525656</v>
@@ -4278,7 +4278,7 @@
             <v>ZA</v>
           </cell>
           <cell r="J9" t="str">
-            <v>Calvin 2011</v>
+            <v>Calvin2011</v>
           </cell>
         </row>
         <row r="10">
@@ -4295,7 +4295,7 @@
             <v>1.1139392249790911</v>
           </cell>
           <cell r="E10">
-            <v>1.3403410595028735</v>
+            <v>1.3370581570459037</v>
           </cell>
           <cell r="F10">
             <v>1.2236660554393917</v>
@@ -4310,7 +4310,7 @@
             <v>ZA</v>
           </cell>
           <cell r="J10" t="str">
-            <v>Calvin 2011</v>
+            <v>Calvin2011</v>
           </cell>
         </row>
         <row r="11">
@@ -4327,7 +4327,7 @@
             <v>1.1342939782548089</v>
           </cell>
           <cell r="E11">
-            <v>1.3387269687270591</v>
+            <v>1.3624787594176615</v>
           </cell>
           <cell r="F11">
             <v>1.2563636877417368</v>
@@ -4342,7 +4342,7 @@
             <v>ZA</v>
           </cell>
           <cell r="J11" t="str">
-            <v>Calvin 2011</v>
+            <v>Calvin2011</v>
           </cell>
         </row>
         <row r="12">
@@ -4359,7 +4359,7 @@
             <v>1.1560252299972122</v>
           </cell>
           <cell r="E12">
-            <v>1.350606551053589</v>
+            <v>1.4316902299447891</v>
           </cell>
           <cell r="F12">
             <v>1.2722882753220093</v>
@@ -4374,7 +4374,7 @@
             <v>ZA</v>
           </cell>
           <cell r="J12" t="str">
-            <v>Calvin 2011</v>
+            <v>Calvin2011</v>
           </cell>
         </row>
         <row r="13">
@@ -4391,7 +4391,7 @@
             <v>1.1797672149428491</v>
           </cell>
           <cell r="E13">
-            <v>1.3693591903438846</v>
+            <v>1.4290585143517762</v>
           </cell>
           <cell r="F13">
             <v>1.245219020840683</v>
@@ -4406,7 +4406,7 @@
             <v>ZA</v>
           </cell>
           <cell r="J13" t="str">
-            <v>Calvin 2011</v>
+            <v>Calvin2011</v>
           </cell>
         </row>
         <row r="14">
@@ -4423,7 +4423,7 @@
             <v>1.2125627265124059</v>
           </cell>
           <cell r="E14">
-            <v>1.4075982660929032</v>
+            <v>1.411057287076307</v>
           </cell>
           <cell r="F14">
             <v>1.3360197031591734</v>
@@ -4438,7 +4438,7 @@
             <v>ZA</v>
           </cell>
           <cell r="J14" t="str">
-            <v>Calvin 2011</v>
+            <v>Calvin2011</v>
           </cell>
         </row>
         <row r="15">
@@ -4455,7 +4455,7 @@
             <v>1.2579174797881238</v>
           </cell>
           <cell r="E15">
-            <v>1.501324121509906</v>
+            <v>1.430470164808008</v>
           </cell>
           <cell r="F15">
             <v>1.4170622080665702</v>
@@ -4470,7 +4470,7 @@
             <v>ZA</v>
           </cell>
           <cell r="J15" t="str">
-            <v>Calvin 2011</v>
+            <v>Calvin2011</v>
           </cell>
         </row>
         <row r="16">
@@ -4487,7 +4487,7 @@
             <v>1.314402704209646</v>
           </cell>
           <cell r="E16">
-            <v>1.5184945407326125</v>
+            <v>1.5078001494712243</v>
           </cell>
           <cell r="F16">
             <v>1.3995427520911294</v>
@@ -4502,7 +4502,7 @@
             <v>ZA</v>
           </cell>
           <cell r="J16" t="str">
-            <v>Calvin 2011</v>
+            <v>Calvin2011</v>
           </cell>
         </row>
         <row r="17">
@@ -4519,7 +4519,7 @@
             <v>1.3844891274045164</v>
           </cell>
           <cell r="E17">
-            <v>1.5981624695740144</v>
+            <v>1.5791353791735665</v>
           </cell>
           <cell r="F17">
             <v>1.4384251849680523</v>
@@ -4534,7 +4534,7 @@
             <v>ZA</v>
           </cell>
           <cell r="J17" t="str">
-            <v>Calvin 2011</v>
+            <v>Calvin2011</v>
           </cell>
         </row>
         <row r="18">
@@ -4551,7 +4551,7 @@
             <v>1.4726303317535545</v>
           </cell>
           <cell r="E18">
-            <v>1.6965749186042138</v>
+            <v>1.5834311139740107</v>
           </cell>
           <cell r="F18">
             <v>1.4686791275267892</v>
@@ -4566,7 +4566,7 @@
             <v>ZA</v>
           </cell>
           <cell r="J18" t="str">
-            <v>Calvin 2011</v>
+            <v>Calvin2011</v>
           </cell>
         </row>
         <row r="19">
@@ -4583,7 +4583,7 @@
             <v>1.576303317535545</v>
           </cell>
           <cell r="E19">
-            <v>1.7562529512365346</v>
+            <v>1.6327508266504545</v>
           </cell>
           <cell r="F19">
             <v>1.5369459119356834</v>
@@ -4598,7 +4598,7 @@
             <v>ZA</v>
           </cell>
           <cell r="J19" t="str">
-            <v>Calvin 2011</v>
+            <v>Calvin2011</v>
           </cell>
         </row>
         <row r="20">
@@ -4615,7 +4615,7 @@
             <v>1.6803038751045443</v>
           </cell>
           <cell r="E20">
-            <v>1.7140554190780692</v>
+            <v>1.5806199554544726</v>
           </cell>
           <cell r="F20">
             <v>1.5126247791683525</v>
@@ -4630,7 +4630,7 @@
             <v>ZA</v>
           </cell>
           <cell r="J20" t="str">
-            <v>Calvin 2011</v>
+            <v>Calvin2011</v>
           </cell>
         </row>
         <row r="21">
@@ -4647,7 +4647,7 @@
             <v>1.7923264566490102</v>
           </cell>
           <cell r="E21">
-            <v>1.655651326002332</v>
+            <v>1.537536704001911</v>
           </cell>
           <cell r="F21">
             <v>1.5133785482256334</v>
@@ -4662,7 +4662,7 @@
             <v>ZA</v>
           </cell>
           <cell r="J21" t="str">
-            <v>Calvin 2011</v>
+            <v>Calvin2011</v>
           </cell>
         </row>
         <row r="22">
@@ -4679,7 +4679,7 @@
             <v>1.9066211318650683</v>
           </cell>
           <cell r="E22">
-            <v>1.6753721408566637</v>
+            <v>1.5565431838533261</v>
           </cell>
           <cell r="F22">
             <v>1.5052918416080747</v>
@@ -4694,7 +4694,7 @@
             <v>ZA</v>
           </cell>
           <cell r="J22" t="str">
-            <v>Calvin 2011</v>
+            <v>Calvin2011</v>
           </cell>
         </row>
       </sheetData>
@@ -4717,7 +4717,7 @@
       <sheetName val="Exergy calcs"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="0"/>
       <sheetData sheetId="1">
         <row r="2">
           <cell r="A2">
@@ -4765,7 +4765,7 @@
             <v>1.0598546016298735</v>
           </cell>
           <cell r="E3">
-            <v>1.049243271788266</v>
+            <v>1.0376879405982591</v>
           </cell>
           <cell r="F3">
             <v>1.0553504171748396</v>
@@ -4797,7 +4797,7 @@
             <v>1.116506736173992</v>
           </cell>
           <cell r="E4">
-            <v>1.0791928743751737</v>
+            <v>1.0707955885023615</v>
           </cell>
           <cell r="F4">
             <v>1.0984891078023766</v>
@@ -4829,7 +4829,7 @@
             <v>1.1702659465214034</v>
           </cell>
           <cell r="E5">
-            <v>1.1059441576535314</v>
+            <v>1.1101549058701556</v>
           </cell>
           <cell r="F5">
             <v>1.131822084103818</v>
@@ -4861,7 +4861,7 @@
             <v>1.2187947499211678</v>
           </cell>
           <cell r="E6">
-            <v>1.1257132484303041</v>
+            <v>1.1285572107002031</v>
           </cell>
           <cell r="F6">
             <v>1.1166623512315266</v>
@@ -4893,7 +4893,7 @@
             <v>1.2542562147244056</v>
           </cell>
           <cell r="E7">
-            <v>1.1207757418060087</v>
+            <v>1.1164267518946909</v>
           </cell>
           <cell r="F7">
             <v>1.1949625842195228</v>
@@ -4925,7 +4925,7 @@
             <v>1.2887861579363036</v>
           </cell>
           <cell r="E8">
-            <v>1.0884299645035702</v>
+            <v>1.1067430954887363</v>
           </cell>
           <cell r="F8">
             <v>1.265522909688287</v>
@@ -4957,7 +4957,7 @@
             <v>1.3288676226816829</v>
           </cell>
           <cell r="E9">
-            <v>1.0967693701882939</v>
+            <v>1.0956347646807536</v>
           </cell>
           <cell r="F9">
             <v>1.3130381249218592</v>
@@ -4989,7 +4989,7 @@
             <v>1.3774051048540374</v>
           </cell>
           <cell r="E10">
-            <v>1.1337100118061223</v>
+            <v>1.126120489587856</v>
           </cell>
           <cell r="F10">
             <v>1.3301716683831304</v>
@@ -5021,7 +5021,7 @@
             <v>1.4293099507913594</v>
           </cell>
           <cell r="E11">
-            <v>1.1607140030438332</v>
+            <v>1.1801172833283424</v>
           </cell>
           <cell r="F11">
             <v>1.400309878998776</v>
@@ -5053,7 +5053,7 @@
             <v>1.4799043020675728</v>
           </cell>
           <cell r="E12">
-            <v>1.2171908200031087</v>
+            <v>1.2346824259441442</v>
           </cell>
           <cell r="F12">
             <v>1.4797842836205422</v>
@@ -5085,7 +5085,7 @@
             <v>1.5290116903066788</v>
           </cell>
           <cell r="E13">
-            <v>1.283558835066958</v>
+            <v>1.3075793820868926</v>
           </cell>
           <cell r="F13">
             <v>1.5509657059675972</v>
@@ -5117,7 +5117,7 @@
             <v>1.5999866925486952</v>
           </cell>
           <cell r="E14">
-            <v>1.4080252965623752</v>
+            <v>1.4026956155027717</v>
           </cell>
           <cell r="F14">
             <v>1.642287298330382</v>
@@ -5149,7 +5149,7 @@
             <v>1.6704930410708447</v>
           </cell>
           <cell r="E15">
-            <v>1.5175964808297548</v>
+            <v>1.4979997675911214</v>
           </cell>
           <cell r="F15">
             <v>1.7630182123296265</v>
@@ -5181,7 +5181,7 @@
             <v>1.769911274014887</v>
           </cell>
           <cell r="E16">
-            <v>1.5716842956517962</v>
+            <v>1.6036207419562249</v>
           </cell>
           <cell r="F16">
             <v>1.8467910217842849</v>
@@ -5213,7 +5213,7 @@
             <v>1.8990427313833096</v>
           </cell>
           <cell r="E17">
-            <v>1.6458238857237517</v>
+            <v>1.6532724007222435</v>
           </cell>
           <cell r="F17">
             <v>1.9015211202007152</v>
@@ -5245,7 +5245,7 @@
             <v>2.065484232116666</v>
           </cell>
           <cell r="E18">
-            <v>1.717856820856833</v>
+            <v>1.7294004390193514</v>
           </cell>
           <cell r="F18">
             <v>1.9837804334929643</v>
@@ -5277,7 +5277,7 @@
             <v>2.2829800590735121</v>
           </cell>
           <cell r="E19">
-            <v>1.7883964032978603</v>
+            <v>1.7897568937332109</v>
           </cell>
           <cell r="F19">
             <v>1.9462941711455051</v>
@@ -5309,7 +5309,7 @@
             <v>2.4182647662083312</v>
           </cell>
           <cell r="E20">
-            <v>1.7941336063839641</v>
+            <v>1.8260589677338577</v>
           </cell>
           <cell r="F20">
             <v>2.0525375507856669</v>
@@ -5341,7 +5341,7 @@
             <v>2.5547037500976364</v>
           </cell>
           <cell r="E21">
-            <v>1.8635175216746698</v>
+            <v>1.8899834246915592</v>
           </cell>
           <cell r="F21">
             <v>2.2461628284231305</v>
@@ -5373,7 +5373,7 @@
             <v>2.6944319887985975</v>
           </cell>
           <cell r="E22">
-            <v>1.9065922194592113</v>
+            <v>1.976029579256867</v>
           </cell>
           <cell r="F22">
             <v>2.7192170244508747</v>
@@ -5393,8 +5393,8 @@
         </row>
       </sheetData>
       <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -5411,7 +5411,7 @@
       <sheetName val="Exergy calcs"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="0"/>
       <sheetData sheetId="1">
         <row r="2">
           <cell r="A2">
@@ -5459,7 +5459,7 @@
             <v>1.0286817340947478</v>
           </cell>
           <cell r="E3">
-            <v>0.9923206837799815</v>
+            <v>1.0033121086200276</v>
           </cell>
           <cell r="F3">
             <v>1.03577726673788</v>
@@ -5491,7 +5491,7 @@
             <v>1.0451808359473445</v>
           </cell>
           <cell r="E4">
-            <v>1.0258154818585306</v>
+            <v>1.0189020330444378</v>
           </cell>
           <cell r="F4">
             <v>1.0670517918372191</v>
@@ -5523,7 +5523,7 @@
             <v>1.0479449851202445</v>
           </cell>
           <cell r="E5">
-            <v>1.0326056463787794</v>
+            <v>1.0378848863983947</v>
           </cell>
           <cell r="F5">
             <v>1.1384492952767526</v>
@@ -5555,7 +5555,7 @@
             <v>1.0470682860130298</v>
           </cell>
           <cell r="E6">
-            <v>1.0676674469765692</v>
+            <v>1.0625750901913893</v>
           </cell>
           <cell r="F6">
             <v>1.1811177098520949</v>
@@ -5587,7 +5587,7 @@
             <v>1.0643931472693637</v>
           </cell>
           <cell r="E7">
-            <v>1.0762276410999878</v>
+            <v>1.0876781311675561</v>
           </cell>
           <cell r="F7">
             <v>1.2237451216322293</v>
@@ -5619,7 +5619,7 @@
             <v>1.09182283707338</v>
           </cell>
           <cell r="E8">
-            <v>1.1451203214814862</v>
+            <v>1.1320499221977611</v>
           </cell>
           <cell r="F8">
             <v>1.3683060315565108</v>
@@ -5651,7 +5651,7 @@
             <v>1.1206413040564089</v>
           </cell>
           <cell r="E9">
-            <v>1.2057762614790537</v>
+            <v>1.1872715086460475</v>
           </cell>
           <cell r="F9">
             <v>1.4185152398016532</v>
@@ -5683,7 +5683,7 @@
             <v>1.1535537145767982</v>
           </cell>
           <cell r="E10">
-            <v>1.2474506450804785</v>
+            <v>1.2494596661144923</v>
           </cell>
           <cell r="F10">
             <v>1.4965058998303231</v>
@@ -5715,7 +5715,7 @@
             <v>1.1887396444944904</v>
           </cell>
           <cell r="E11">
-            <v>1.3427875426021263</v>
+            <v>1.2908758337952513</v>
           </cell>
           <cell r="F11">
             <v>1.5560989999636801</v>
@@ -5747,7 +5747,7 @@
             <v>1.2378857342019893</v>
           </cell>
           <cell r="E12">
-            <v>1.4046771040381612</v>
+            <v>1.3750116062118418</v>
           </cell>
           <cell r="F12">
             <v>1.6635605320156388</v>
@@ -5779,7 +5779,7 @@
             <v>1.2994879219282018</v>
           </cell>
           <cell r="E13">
-            <v>1.4662256242124556</v>
+            <v>1.4447440859500611</v>
           </cell>
           <cell r="F13">
             <v>1.8190034559936956</v>
@@ -5811,7 +5811,7 @@
             <v>1.3727713879728678</v>
           </cell>
           <cell r="E14">
-            <v>1.5669527354415114</v>
+            <v>1.5333168827828205</v>
           </cell>
           <cell r="F14">
             <v>1.9151848972041365</v>
@@ -5843,7 +5843,7 @@
             <v>1.4523552910265691</v>
           </cell>
           <cell r="E15">
-            <v>1.7123166508885288</v>
+            <v>1.6513280651642879</v>
           </cell>
           <cell r="F15">
             <v>1.988985776194522</v>
@@ -5875,7 +5875,7 @@
             <v>1.5352797662135713</v>
           </cell>
           <cell r="E16">
-            <v>1.7569037569931252</v>
+            <v>1.6936795889934797</v>
           </cell>
           <cell r="F16">
             <v>2.2734187837172928</v>
@@ -5907,7 +5907,7 @@
             <v>1.618542052065739</v>
           </cell>
           <cell r="E17">
-            <v>1.7594397758824338</v>
+            <v>1.7068970430814494</v>
           </cell>
           <cell r="F17">
             <v>2.3782745936048397</v>
@@ -5939,7 +5939,7 @@
             <v>1.7074130673744605</v>
           </cell>
           <cell r="E18">
-            <v>1.8044561053690826</v>
+            <v>1.7243467380143345</v>
           </cell>
           <cell r="F18">
             <v>2.4357701852027778</v>
@@ -5971,7 +5971,7 @@
             <v>1.8001715863696077</v>
           </cell>
           <cell r="E19">
-            <v>1.7369485759342249</v>
+            <v>1.671027329007184</v>
           </cell>
           <cell r="F19">
             <v>2.5228589645233384</v>
@@ -6003,7 +6003,7 @@
             <v>1.8938657872865223</v>
           </cell>
           <cell r="E20">
-            <v>1.7804433072068904</v>
+            <v>1.6821511333211596</v>
           </cell>
           <cell r="F20">
             <v>2.7902337269664645</v>
@@ -6035,7 +6035,7 @@
             <v>1.9875921606477385</v>
           </cell>
           <cell r="E21">
-            <v>1.8469810667781668</v>
+            <v>1.6917742808198715</v>
           </cell>
           <cell r="F21">
             <v>2.809955102096009</v>
@@ -6067,7 +6067,7 @@
             <v>2.0860746936915198</v>
           </cell>
           <cell r="E22">
-            <v>1.8675789761098966</v>
+            <v>1.7317523832170316</v>
           </cell>
           <cell r="F22">
             <v>3.107350258445607</v>
@@ -6087,8 +6087,8 @@
         </row>
       </sheetData>
       <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -6105,7 +6105,7 @@
       <sheetName val="Exergy calcs"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="0"/>
       <sheetData sheetId="1">
         <row r="2">
           <cell r="A2">
@@ -6153,7 +6153,7 @@
             <v>1.0783058575938267</v>
           </cell>
           <cell r="E3">
-            <v>1.0210508656820274</v>
+            <v>1.0367182268975108</v>
           </cell>
           <cell r="F3">
             <v>1.0340047944777087</v>
@@ -6185,7 +6185,7 @@
             <v>1.1341634514205541</v>
           </cell>
           <cell r="E4">
-            <v>1.0556153313366927</v>
+            <v>1.0720661216957412</v>
           </cell>
           <cell r="F4">
             <v>1.0692739180023667</v>
@@ -6217,7 +6217,7 @@
             <v>1.1878288319887758</v>
           </cell>
           <cell r="E5">
-            <v>1.1099907940373888</v>
+            <v>1.1082826130812979</v>
           </cell>
           <cell r="F5">
             <v>1.0375743391680856</v>
@@ -6249,7 +6249,7 @@
             <v>1.2178183093651351</v>
           </cell>
           <cell r="E6">
-            <v>1.143580093612782</v>
+            <v>1.1351728279061144</v>
           </cell>
           <cell r="F6">
             <v>1.0429279831211073</v>
@@ -6281,7 +6281,7 @@
             <v>1.2428095405121009</v>
           </cell>
           <cell r="E7">
-            <v>1.1756384700676845</v>
+            <v>1.1640850070012463</v>
           </cell>
           <cell r="F7">
             <v>1.067160388810108</v>
@@ -6313,7 +6313,7 @@
             <v>1.2663977551736232</v>
           </cell>
           <cell r="E8">
-            <v>1.206546229055788</v>
+            <v>1.2014315300214575</v>
           </cell>
           <cell r="F8">
             <v>1.0436917895936202</v>
@@ -6345,7 +6345,7 @@
             <v>1.3040161346895827</v>
           </cell>
           <cell r="E9">
-            <v>1.2210962860108654</v>
+            <v>1.232593595417365</v>
           </cell>
           <cell r="F9">
             <v>1.0961258261618216</v>
@@ -6377,7 +6377,7 @@
             <v>1.3468081374956156</v>
           </cell>
           <cell r="E10">
-            <v>1.2515828710931032</v>
+            <v>1.2654602066338621</v>
           </cell>
           <cell r="F10">
             <v>1.1225864050460994</v>
@@ -6409,7 +6409,7 @@
             <v>1.3944230094703614</v>
           </cell>
           <cell r="E11">
-            <v>1.2832842687413721</v>
+            <v>1.2931681655671592</v>
           </cell>
           <cell r="F11">
             <v>1.124068541404684</v>
@@ -6441,7 +6441,7 @@
             <v>1.4558049807085234</v>
           </cell>
           <cell r="E12">
-            <v>1.3164204285711589</v>
+            <v>1.3280146578118128</v>
           </cell>
           <cell r="F12">
             <v>1.2116332758164539</v>
@@ -6473,7 +6473,7 @@
             <v>1.5255173623290075</v>
           </cell>
           <cell r="E13">
-            <v>1.3684776113712027</v>
+            <v>1.3898522836711655</v>
           </cell>
           <cell r="F13">
             <v>1.2681756403645339</v>
@@ -6505,7 +6505,7 @@
             <v>1.6142581550333217</v>
           </cell>
           <cell r="E14">
-            <v>1.4229926061957845</v>
+            <v>1.4327510497077038</v>
           </cell>
           <cell r="F14">
             <v>1.2817801916504126</v>
@@ -6537,7 +6537,7 @@
             <v>1.7172044896527534</v>
           </cell>
           <cell r="E15">
-            <v>1.4616215628210345</v>
+            <v>1.4824489763374917</v>
           </cell>
           <cell r="F15">
             <v>1.3303358394122207</v>
@@ -6569,7 +6569,7 @@
             <v>1.8532094002104524</v>
           </cell>
           <cell r="E16">
-            <v>1.5020071213170048</v>
+            <v>1.5324909718893391</v>
           </cell>
           <cell r="F16">
             <v>1.4046100612284109</v>
@@ -6601,7 +6601,7 @@
             <v>2.0208698702209751</v>
           </cell>
           <cell r="E17">
-            <v>1.5442689594453047</v>
+            <v>1.5468078837584009</v>
           </cell>
           <cell r="F17">
             <v>1.4330854124506951</v>
@@ -6633,7 +6633,7 @@
             <v>2.2198351455629606</v>
           </cell>
           <cell r="E18">
-            <v>1.5885418403996812</v>
+            <v>1.6281584008640875</v>
           </cell>
           <cell r="F18">
             <v>1.5627634799051398</v>
@@ -6665,7 +6665,7 @@
             <v>2.4314275692739389</v>
           </cell>
           <cell r="E19">
-            <v>1.6349385181151996</v>
+            <v>1.6658599441961892</v>
           </cell>
           <cell r="F19">
             <v>1.6284782451239013</v>
@@ -6697,7 +6697,7 @@
             <v>2.6652928796913362</v>
           </cell>
           <cell r="E20">
-            <v>1.6835627726288354</v>
+            <v>1.7130039249835767</v>
           </cell>
           <cell r="F20">
             <v>1.6888896525810746</v>
@@ -6729,7 +6729,7 @@
             <v>2.9149421255699752</v>
           </cell>
           <cell r="E21">
-            <v>1.7344853120686496</v>
+            <v>1.7541696811874952</v>
           </cell>
           <cell r="F21">
             <v>1.6680680933119416</v>
@@ -6761,7 +6761,7 @@
             <v>3.1830059628200633</v>
           </cell>
           <cell r="E22">
-            <v>1.7877585486411658</v>
+            <v>1.7970941883839631</v>
           </cell>
           <cell r="F22">
             <v>1.8858194322791211</v>
@@ -6781,8 +6781,8 @@
         </row>
       </sheetData>
       <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -6847,7 +6847,7 @@
             <v>0.96924639152825121</v>
           </cell>
           <cell r="E3">
-            <v>1.0253503606606469</v>
+            <v>1.0224901654943095</v>
           </cell>
           <cell r="F3">
             <v>1.0372902442435501</v>
@@ -6879,7 +6879,7 @@
             <v>0.95655327482410968</v>
           </cell>
           <cell r="E4">
-            <v>1.0538740327847183</v>
+            <v>1.0399701099499545</v>
           </cell>
           <cell r="F4">
             <v>0.99283416815065528</v>
@@ -6911,7 +6911,7 @@
             <v>0.93138463770218327</v>
           </cell>
           <cell r="E5">
-            <v>1.0973728039159725</v>
+            <v>1.0777929567401658</v>
           </cell>
           <cell r="F5">
             <v>0.96226552654774133</v>
@@ -6943,7 +6943,7 @@
             <v>0.91796620004351925</v>
           </cell>
           <cell r="E6">
-            <v>1.126011730223049</v>
+            <v>1.1140511839801894</v>
           </cell>
           <cell r="F6">
             <v>0.97640745714480581</v>
@@ -6975,7 +6975,7 @@
             <v>0.91550010879814314</v>
           </cell>
           <cell r="E7">
-            <v>1.2100048752017798</v>
+            <v>1.1875048984137102</v>
           </cell>
           <cell r="F7">
             <v>0.94601991154713516</v>
@@ -7007,7 +7007,7 @@
             <v>0.92913614274316381</v>
           </cell>
           <cell r="E8">
-            <v>1.2621311954601659</v>
+            <v>1.2305758921930401</v>
           </cell>
           <cell r="F8">
             <v>1.0127519539095122</v>
@@ -7039,7 +7039,7 @@
             <v>0.96503952999202147</v>
           </cell>
           <cell r="E9">
-            <v>1.3351105243839876</v>
+            <v>1.302664022117958</v>
           </cell>
           <cell r="F9">
             <v>0.98049396767421726</v>
@@ -7071,7 +7071,7 @@
             <v>1.0200913904402698</v>
           </cell>
           <cell r="E10">
-            <v>1.3520695749730507</v>
+            <v>1.3344645592351276</v>
           </cell>
           <cell r="F10">
             <v>0.97569047936520592</v>
@@ -7103,7 +7103,7 @@
             <v>1.0180604917676073</v>
           </cell>
           <cell r="E11">
-            <v>1.3869343489141379</v>
+            <v>1.355101232872514</v>
           </cell>
           <cell r="F11">
             <v>0.97545030108404673</v>
@@ -7135,7 +7135,7 @@
             <v>1.0260390222673532</v>
           </cell>
           <cell r="E12">
-            <v>1.3800954400339227</v>
+            <v>1.3517817406304078</v>
           </cell>
           <cell r="F12">
             <v>1.0126536105257817</v>
@@ -7167,7 +7167,7 @@
             <v>1.0379342859215204</v>
           </cell>
           <cell r="E13">
-            <v>1.4069868802031238</v>
+            <v>1.3907644608391989</v>
           </cell>
           <cell r="F13">
             <v>1.0295376485352523</v>
@@ -7199,7 +7199,7 @@
             <v>1.0541089432073694</v>
           </cell>
           <cell r="E14">
-            <v>1.4183370759572067</v>
+            <v>1.4033972482347783</v>
           </cell>
           <cell r="F14">
             <v>1.0578078265415378</v>
@@ -7231,7 +7231,7 @@
             <v>1.0658591426706319</v>
           </cell>
           <cell r="E15">
-            <v>1.4512935001605018</v>
+            <v>1.4318123720670304</v>
           </cell>
           <cell r="F15">
             <v>1.0648635894119554</v>
@@ -7263,7 +7263,7 @@
             <v>1.0818887357655762</v>
           </cell>
           <cell r="E16">
-            <v>1.4644390379448708</v>
+            <v>1.4564504375255525</v>
           </cell>
           <cell r="F16">
             <v>1.1145715820582243</v>
@@ -7295,7 +7295,7 @@
             <v>1.1066221803147893</v>
           </cell>
           <cell r="E17">
-            <v>1.5012008832340635</v>
+            <v>1.4949043807496252</v>
           </cell>
           <cell r="F17">
             <v>1.1729546519188956</v>
@@ -7327,7 +7327,7 @@
             <v>1.1382461739319649</v>
           </cell>
           <cell r="E18">
-            <v>1.5402035223111452</v>
+            <v>1.5320191060408039</v>
           </cell>
           <cell r="F18">
             <v>1.1678285269002644</v>
@@ -7359,7 +7359,7 @@
             <v>1.1745122216580837</v>
           </cell>
           <cell r="E19">
-            <v>1.5816270976723197</v>
+            <v>1.5725131433126012</v>
           </cell>
           <cell r="F19">
             <v>1.1142506951948152</v>
@@ -7391,7 +7391,7 @@
             <v>1.2152027272067889</v>
           </cell>
           <cell r="E20">
-            <v>1.6255938762458619</v>
+            <v>1.6215594097703909</v>
           </cell>
           <cell r="F20">
             <v>1.1775631819612329</v>
@@ -7423,7 +7423,7 @@
             <v>1.2668455791687823</v>
           </cell>
           <cell r="E21">
-            <v>1.6514862299396258</v>
+            <v>1.7196442344046197</v>
           </cell>
           <cell r="F21">
             <v>1.2642839456164883</v>
@@ -7455,7 +7455,7 @@
             <v>1.3440197287299631</v>
           </cell>
           <cell r="E22">
-            <v>1.7215693266011487</v>
+            <v>1.7738033236619906</v>
           </cell>
           <cell r="F22">
             <v>1.3328208853352348</v>
@@ -7474,6 +7474,7 @@
           </cell>
         </row>
       </sheetData>
+      <sheetData sheetId="2" refreshError="1"/>
       <sheetData sheetId="3"/>
       <sheetData sheetId="4"/>
     </sheetDataSet>
@@ -7806,7 +7807,7 @@
   <dimension ref="A1:J223"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="560" topLeftCell="A203" activePane="bottomLeft"/>
+      <pane ySplit="560" topLeftCell="A36" activePane="bottomLeft"/>
       <selection activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A223" sqref="A223"/>
     </sheetView>
@@ -8841,7 +8842,7 @@
       </c>
       <c r="E25" s="2">
         <f>[1]USData!E25</f>
-        <v>1.353821572975088</v>
+        <v>1.3538215729750882</v>
       </c>
       <c r="F25" s="2">
         <f>[1]USData!F25</f>
@@ -8925,7 +8926,7 @@
       </c>
       <c r="E27" s="2">
         <f>[1]USData!E27</f>
-        <v>1.3900863005956263</v>
+        <v>1.3900863005956265</v>
       </c>
       <c r="F27" s="2">
         <f>[1]USData!F27</f>
@@ -9009,7 +9010,7 @@
       </c>
       <c r="E29" s="2">
         <f>[1]USData!E29</f>
-        <v>1.4253238989609147</v>
+        <v>1.4252423807660537</v>
       </c>
       <c r="F29" s="2">
         <f>[1]USData!F29</f>
@@ -9051,7 +9052,7 @@
       </c>
       <c r="E30" s="2">
         <f>[1]USData!E30</f>
-        <v>1.4099386983174644</v>
+        <v>1.4100365201512979</v>
       </c>
       <c r="F30" s="2">
         <f>[1]USData!F30</f>
@@ -9093,7 +9094,7 @@
       </c>
       <c r="E31" s="2">
         <f>[1]USData!E31</f>
-        <v>1.3323170731707317</v>
+        <v>1.3320833876787965</v>
       </c>
       <c r="F31" s="2">
         <f>[1]USData!F31</f>
@@ -9135,7 +9136,7 @@
       </c>
       <c r="E32" s="2">
         <f>[1]USData!E32</f>
-        <v>1.3317627494456763</v>
+        <v>1.3321431676883613</v>
       </c>
       <c r="F32" s="2">
         <f>[1]USData!F32</f>
@@ -9177,7 +9178,7 @@
       </c>
       <c r="E33" s="2">
         <f>[1]USData!E33</f>
-        <v>1.3741821007782271</v>
+        <v>1.3521966436241903</v>
       </c>
       <c r="F33" s="2">
         <f>[1]USData!F33</f>
@@ -11949,7 +11950,7 @@
       </c>
       <c r="E99" s="2">
         <f>[4]CNData!E3</f>
-        <v>1.025828510517504</v>
+        <v>1.0178691150298789</v>
       </c>
       <c r="F99" s="2">
         <f>[4]CNData!F3</f>
@@ -11991,7 +11992,7 @@
       </c>
       <c r="E100" s="2">
         <f>[4]CNData!E4</f>
-        <v>1.0376896829396873</v>
+        <v>1.0326830865914762</v>
       </c>
       <c r="F100" s="2">
         <f>[4]CNData!F4</f>
@@ -12033,7 +12034,7 @@
       </c>
       <c r="E101" s="2">
         <f>[4]CNData!E5</f>
-        <v>1.0500601886449963</v>
+        <v>1.0455996349512124</v>
       </c>
       <c r="F101" s="2">
         <f>[4]CNData!F5</f>
@@ -12075,7 +12076,7 @@
       </c>
       <c r="E102" s="2">
         <f>[4]CNData!E6</f>
-        <v>1.0615313936827389</v>
+        <v>1.0567805903326029</v>
       </c>
       <c r="F102" s="2">
         <f>[4]CNData!F6</f>
@@ -12117,7 +12118,7 @@
       </c>
       <c r="E103" s="2">
         <f>[4]CNData!E7</f>
-        <v>1.0727162591170047</v>
+        <v>1.0705089171150399</v>
       </c>
       <c r="F103" s="2">
         <f>[4]CNData!F7</f>
@@ -12159,7 +12160,7 @@
       </c>
       <c r="E104" s="2">
         <f>[4]CNData!E8</f>
-        <v>1.0837513469125288</v>
+        <v>1.0855105334223953</v>
       </c>
       <c r="F104" s="2">
         <f>[4]CNData!F8</f>
@@ -12201,7 +12202,7 @@
       </c>
       <c r="E105" s="2">
         <f>[4]CNData!E9</f>
-        <v>1.0944003938069702</v>
+        <v>1.098663887061381</v>
       </c>
       <c r="F105" s="2">
         <f>[4]CNData!F9</f>
@@ -12243,7 +12244,7 @@
       </c>
       <c r="E106" s="2">
         <f>[4]CNData!E10</f>
-        <v>1.1039174170433839</v>
+        <v>1.1142496548803333</v>
       </c>
       <c r="F106" s="2">
         <f>[4]CNData!F10</f>
@@ -12285,7 +12286,7 @@
       </c>
       <c r="E107" s="2">
         <f>[4]CNData!E11</f>
-        <v>1.1276859801371437</v>
+        <v>1.131015892925423</v>
       </c>
       <c r="F107" s="2">
         <f>[4]CNData!F11</f>
@@ -12327,7 +12328,7 @@
       </c>
       <c r="E108" s="2">
         <f>[4]CNData!E12</f>
-        <v>1.1205569990209538</v>
+        <v>1.142997759030947</v>
       </c>
       <c r="F108" s="2">
         <f>[4]CNData!F12</f>
@@ -12369,7 +12370,7 @@
       </c>
       <c r="E109" s="2">
         <f>[4]CNData!E13</f>
-        <v>1.1431311323141213</v>
+        <v>1.155848264812064</v>
       </c>
       <c r="F109" s="2">
         <f>[4]CNData!F13</f>
@@ -12411,7 +12412,7 @@
       </c>
       <c r="E110" s="2">
         <f>[4]CNData!E14</f>
-        <v>1.1654086471462513</v>
+        <v>1.168481752026193</v>
       </c>
       <c r="F110" s="2">
         <f>[4]CNData!F14</f>
@@ -12453,7 +12454,7 @@
       </c>
       <c r="E111" s="2">
         <f>[4]CNData!E15</f>
-        <v>1.15629138497367</v>
+        <v>1.1779171478102899</v>
       </c>
       <c r="F111" s="2">
         <f>[4]CNData!F15</f>
@@ -12495,7 +12496,7 @@
       </c>
       <c r="E112" s="2">
         <f>[4]CNData!E16</f>
-        <v>1.17821720919724</v>
+        <v>1.1900291761365198</v>
       </c>
       <c r="F112" s="2">
         <f>[4]CNData!F16</f>
@@ -12537,7 +12538,7 @@
       </c>
       <c r="E113" s="2">
         <f>[4]CNData!E17</f>
-        <v>1.2000044028108472</v>
+        <v>1.1992960303175253</v>
       </c>
       <c r="F113" s="2">
         <f>[4]CNData!F17</f>
@@ -12579,7 +12580,7 @@
       </c>
       <c r="E114" s="2">
         <f>[4]CNData!E18</f>
-        <v>1.2062880828655347</v>
+        <v>1.2093135026735413</v>
       </c>
       <c r="F114" s="2">
         <f>[4]CNData!F18</f>
@@ -12621,7 +12622,7 @@
       </c>
       <c r="E115" s="2">
         <f>[4]CNData!E19</f>
-        <v>1.210779484188824</v>
+        <v>1.2065325839291203</v>
       </c>
       <c r="F115" s="2">
         <f>[4]CNData!F19</f>
@@ -12663,7 +12664,7 @@
       </c>
       <c r="E116" s="2">
         <f>[4]CNData!E20</f>
-        <v>1.1946446114165401</v>
+        <v>1.210440022781649</v>
       </c>
       <c r="F116" s="2">
         <f>[4]CNData!F20</f>
@@ -12705,7 +12706,7 @@
       </c>
       <c r="E117" s="2">
         <f>[4]CNData!E21</f>
-        <v>1.2004276970273946</v>
+        <v>1.2143930907361127</v>
       </c>
       <c r="F117" s="2">
         <f>[4]CNData!F21</f>
@@ -12747,7 +12748,7 @@
       </c>
       <c r="E118" s="2">
         <f>[4]CNData!E22</f>
-        <v>1.2060851609182306</v>
+        <v>1.2239513102511816</v>
       </c>
       <c r="F118" s="2">
         <f>[4]CNData!F22</f>
@@ -12809,7 +12810,7 @@
       </c>
       <c r="J119" s="1" t="str">
         <f>[5]ZAData!J2</f>
-        <v>Calvin 2011</v>
+        <v>Calvin2011</v>
       </c>
     </row>
     <row r="120" spans="1:10">
@@ -12831,7 +12832,7 @@
       </c>
       <c r="E120" s="2">
         <f>[5]ZAData!E3</f>
-        <v>1.0210844828674435</v>
+        <v>1.0431185657854123</v>
       </c>
       <c r="F120" s="2">
         <f>[5]ZAData!F3</f>
@@ -12851,7 +12852,7 @@
       </c>
       <c r="J120" s="1" t="str">
         <f>[5]ZAData!J3</f>
-        <v>Calvin 2011</v>
+        <v>Calvin2011</v>
       </c>
     </row>
     <row r="121" spans="1:10">
@@ -12873,7 +12874,7 @@
       </c>
       <c r="E121" s="2">
         <f>[5]ZAData!E4</f>
-        <v>1.0596971479482411</v>
+        <v>1.0574888746154401</v>
       </c>
       <c r="F121" s="2">
         <f>[5]ZAData!F4</f>
@@ -12893,7 +12894,7 @@
       </c>
       <c r="J121" s="1" t="str">
         <f>[5]ZAData!J4</f>
-        <v>Calvin 2011</v>
+        <v>Calvin2011</v>
       </c>
     </row>
     <row r="122" spans="1:10">
@@ -12915,7 +12916,7 @@
       </c>
       <c r="E122" s="2">
         <f>[5]ZAData!E5</f>
-        <v>1.1703636849475125</v>
+        <v>1.1799696229951748</v>
       </c>
       <c r="F122" s="2">
         <f>[5]ZAData!F5</f>
@@ -12935,7 +12936,7 @@
       </c>
       <c r="J122" s="1" t="str">
         <f>[5]ZAData!J5</f>
-        <v>Calvin 2011</v>
+        <v>Calvin2011</v>
       </c>
     </row>
     <row r="123" spans="1:10">
@@ -12957,7 +12958,7 @@
       </c>
       <c r="E123" s="2">
         <f>[5]ZAData!E6</f>
-        <v>1.2756746171943205</v>
+        <v>1.2732863978279441</v>
       </c>
       <c r="F123" s="2">
         <f>[5]ZAData!F6</f>
@@ -12977,7 +12978,7 @@
       </c>
       <c r="J123" s="1" t="str">
         <f>[5]ZAData!J6</f>
-        <v>Calvin 2011</v>
+        <v>Calvin2011</v>
       </c>
     </row>
     <row r="124" spans="1:10">
@@ -12999,7 +13000,7 @@
       </c>
       <c r="E124" s="2">
         <f>[5]ZAData!E7</f>
-        <v>1.2422655511589069</v>
+        <v>1.2573109473776538</v>
       </c>
       <c r="F124" s="2">
         <f>[5]ZAData!F7</f>
@@ -13019,7 +13020,7 @@
       </c>
       <c r="J124" s="1" t="str">
         <f>[5]ZAData!J7</f>
-        <v>Calvin 2011</v>
+        <v>Calvin2011</v>
       </c>
     </row>
     <row r="125" spans="1:10">
@@ -13041,7 +13042,7 @@
       </c>
       <c r="E125" s="2">
         <f>[5]ZAData!E8</f>
-        <v>1.2908777646168526</v>
+        <v>1.2752286086734368</v>
       </c>
       <c r="F125" s="2">
         <f>[5]ZAData!F8</f>
@@ -13061,7 +13062,7 @@
       </c>
       <c r="J125" s="1" t="str">
         <f>[5]ZAData!J8</f>
-        <v>Calvin 2011</v>
+        <v>Calvin2011</v>
       </c>
     </row>
     <row r="126" spans="1:10">
@@ -13083,7 +13084,7 @@
       </c>
       <c r="E126" s="2">
         <f>[5]ZAData!E9</f>
-        <v>1.2885477134940848</v>
+        <v>1.2903948686660907</v>
       </c>
       <c r="F126" s="2">
         <f>[5]ZAData!F9</f>
@@ -13103,7 +13104,7 @@
       </c>
       <c r="J126" s="1" t="str">
         <f>[5]ZAData!J9</f>
-        <v>Calvin 2011</v>
+        <v>Calvin2011</v>
       </c>
     </row>
     <row r="127" spans="1:10">
@@ -13125,7 +13126,7 @@
       </c>
       <c r="E127" s="2">
         <f>[5]ZAData!E10</f>
-        <v>1.3403410595028735</v>
+        <v>1.3370581570459037</v>
       </c>
       <c r="F127" s="2">
         <f>[5]ZAData!F10</f>
@@ -13145,7 +13146,7 @@
       </c>
       <c r="J127" s="1" t="str">
         <f>[5]ZAData!J10</f>
-        <v>Calvin 2011</v>
+        <v>Calvin2011</v>
       </c>
     </row>
     <row r="128" spans="1:10">
@@ -13167,7 +13168,7 @@
       </c>
       <c r="E128" s="2">
         <f>[5]ZAData!E11</f>
-        <v>1.3387269687270591</v>
+        <v>1.3624787594176615</v>
       </c>
       <c r="F128" s="2">
         <f>[5]ZAData!F11</f>
@@ -13187,7 +13188,7 @@
       </c>
       <c r="J128" s="1" t="str">
         <f>[5]ZAData!J11</f>
-        <v>Calvin 2011</v>
+        <v>Calvin2011</v>
       </c>
     </row>
     <row r="129" spans="1:10">
@@ -13209,7 +13210,7 @@
       </c>
       <c r="E129" s="2">
         <f>[5]ZAData!E12</f>
-        <v>1.350606551053589</v>
+        <v>1.4316902299447891</v>
       </c>
       <c r="F129" s="2">
         <f>[5]ZAData!F12</f>
@@ -13229,7 +13230,7 @@
       </c>
       <c r="J129" s="1" t="str">
         <f>[5]ZAData!J12</f>
-        <v>Calvin 2011</v>
+        <v>Calvin2011</v>
       </c>
     </row>
     <row r="130" spans="1:10">
@@ -13251,7 +13252,7 @@
       </c>
       <c r="E130" s="2">
         <f>[5]ZAData!E13</f>
-        <v>1.3693591903438846</v>
+        <v>1.4290585143517762</v>
       </c>
       <c r="F130" s="2">
         <f>[5]ZAData!F13</f>
@@ -13271,7 +13272,7 @@
       </c>
       <c r="J130" s="1" t="str">
         <f>[5]ZAData!J13</f>
-        <v>Calvin 2011</v>
+        <v>Calvin2011</v>
       </c>
     </row>
     <row r="131" spans="1:10">
@@ -13293,7 +13294,7 @@
       </c>
       <c r="E131" s="2">
         <f>[5]ZAData!E14</f>
-        <v>1.4075982660929032</v>
+        <v>1.411057287076307</v>
       </c>
       <c r="F131" s="2">
         <f>[5]ZAData!F14</f>
@@ -13313,7 +13314,7 @@
       </c>
       <c r="J131" s="1" t="str">
         <f>[5]ZAData!J14</f>
-        <v>Calvin 2011</v>
+        <v>Calvin2011</v>
       </c>
     </row>
     <row r="132" spans="1:10">
@@ -13335,7 +13336,7 @@
       </c>
       <c r="E132" s="2">
         <f>[5]ZAData!E15</f>
-        <v>1.501324121509906</v>
+        <v>1.430470164808008</v>
       </c>
       <c r="F132" s="2">
         <f>[5]ZAData!F15</f>
@@ -13355,7 +13356,7 @@
       </c>
       <c r="J132" s="1" t="str">
         <f>[5]ZAData!J15</f>
-        <v>Calvin 2011</v>
+        <v>Calvin2011</v>
       </c>
     </row>
     <row r="133" spans="1:10">
@@ -13377,7 +13378,7 @@
       </c>
       <c r="E133" s="2">
         <f>[5]ZAData!E16</f>
-        <v>1.5184945407326125</v>
+        <v>1.5078001494712243</v>
       </c>
       <c r="F133" s="2">
         <f>[5]ZAData!F16</f>
@@ -13397,7 +13398,7 @@
       </c>
       <c r="J133" s="1" t="str">
         <f>[5]ZAData!J16</f>
-        <v>Calvin 2011</v>
+        <v>Calvin2011</v>
       </c>
     </row>
     <row r="134" spans="1:10">
@@ -13419,7 +13420,7 @@
       </c>
       <c r="E134" s="2">
         <f>[5]ZAData!E17</f>
-        <v>1.5981624695740144</v>
+        <v>1.5791353791735665</v>
       </c>
       <c r="F134" s="2">
         <f>[5]ZAData!F17</f>
@@ -13439,7 +13440,7 @@
       </c>
       <c r="J134" s="1" t="str">
         <f>[5]ZAData!J17</f>
-        <v>Calvin 2011</v>
+        <v>Calvin2011</v>
       </c>
     </row>
     <row r="135" spans="1:10">
@@ -13461,7 +13462,7 @@
       </c>
       <c r="E135" s="2">
         <f>[5]ZAData!E18</f>
-        <v>1.6965749186042138</v>
+        <v>1.5834311139740107</v>
       </c>
       <c r="F135" s="2">
         <f>[5]ZAData!F18</f>
@@ -13481,7 +13482,7 @@
       </c>
       <c r="J135" s="1" t="str">
         <f>[5]ZAData!J18</f>
-        <v>Calvin 2011</v>
+        <v>Calvin2011</v>
       </c>
     </row>
     <row r="136" spans="1:10">
@@ -13503,7 +13504,7 @@
       </c>
       <c r="E136" s="2">
         <f>[5]ZAData!E19</f>
-        <v>1.7562529512365346</v>
+        <v>1.6327508266504545</v>
       </c>
       <c r="F136" s="2">
         <f>[5]ZAData!F19</f>
@@ -13523,7 +13524,7 @@
       </c>
       <c r="J136" s="1" t="str">
         <f>[5]ZAData!J19</f>
-        <v>Calvin 2011</v>
+        <v>Calvin2011</v>
       </c>
     </row>
     <row r="137" spans="1:10">
@@ -13545,7 +13546,7 @@
       </c>
       <c r="E137" s="2">
         <f>[5]ZAData!E20</f>
-        <v>1.7140554190780692</v>
+        <v>1.5806199554544726</v>
       </c>
       <c r="F137" s="2">
         <f>[5]ZAData!F20</f>
@@ -13565,7 +13566,7 @@
       </c>
       <c r="J137" s="1" t="str">
         <f>[5]ZAData!J20</f>
-        <v>Calvin 2011</v>
+        <v>Calvin2011</v>
       </c>
     </row>
     <row r="138" spans="1:10">
@@ -13587,7 +13588,7 @@
       </c>
       <c r="E138" s="2">
         <f>[5]ZAData!E21</f>
-        <v>1.655651326002332</v>
+        <v>1.537536704001911</v>
       </c>
       <c r="F138" s="2">
         <f>[5]ZAData!F21</f>
@@ -13607,7 +13608,7 @@
       </c>
       <c r="J138" s="1" t="str">
         <f>[5]ZAData!J21</f>
-        <v>Calvin 2011</v>
+        <v>Calvin2011</v>
       </c>
     </row>
     <row r="139" spans="1:10">
@@ -13629,7 +13630,7 @@
       </c>
       <c r="E139" s="2">
         <f>[5]ZAData!E22</f>
-        <v>1.6753721408566637</v>
+        <v>1.5565431838533261</v>
       </c>
       <c r="F139" s="2">
         <f>[5]ZAData!F22</f>
@@ -13649,7 +13650,7 @@
       </c>
       <c r="J139" s="1" t="str">
         <f>[5]ZAData!J22</f>
-        <v>Calvin 2011</v>
+        <v>Calvin2011</v>
       </c>
     </row>
     <row r="140" spans="1:10">
@@ -13713,7 +13714,7 @@
       </c>
       <c r="E141" s="2">
         <f>[6]SAData!E3</f>
-        <v>1.049243271788266</v>
+        <v>1.0376879405982591</v>
       </c>
       <c r="F141" s="2">
         <f>[6]SAData!F3</f>
@@ -13755,7 +13756,7 @@
       </c>
       <c r="E142" s="2">
         <f>[6]SAData!E4</f>
-        <v>1.0791928743751737</v>
+        <v>1.0707955885023615</v>
       </c>
       <c r="F142" s="2">
         <f>[6]SAData!F4</f>
@@ -13797,7 +13798,7 @@
       </c>
       <c r="E143" s="2">
         <f>[6]SAData!E5</f>
-        <v>1.1059441576535314</v>
+        <v>1.1101549058701556</v>
       </c>
       <c r="F143" s="2">
         <f>[6]SAData!F5</f>
@@ -13839,7 +13840,7 @@
       </c>
       <c r="E144" s="2">
         <f>[6]SAData!E6</f>
-        <v>1.1257132484303041</v>
+        <v>1.1285572107002031</v>
       </c>
       <c r="F144" s="2">
         <f>[6]SAData!F6</f>
@@ -13881,7 +13882,7 @@
       </c>
       <c r="E145" s="2">
         <f>[6]SAData!E7</f>
-        <v>1.1207757418060087</v>
+        <v>1.1164267518946909</v>
       </c>
       <c r="F145" s="2">
         <f>[6]SAData!F7</f>
@@ -13923,7 +13924,7 @@
       </c>
       <c r="E146" s="2">
         <f>[6]SAData!E8</f>
-        <v>1.0884299645035702</v>
+        <v>1.1067430954887363</v>
       </c>
       <c r="F146" s="2">
         <f>[6]SAData!F8</f>
@@ -13965,7 +13966,7 @@
       </c>
       <c r="E147" s="2">
         <f>[6]SAData!E9</f>
-        <v>1.0967693701882939</v>
+        <v>1.0956347646807536</v>
       </c>
       <c r="F147" s="2">
         <f>[6]SAData!F9</f>
@@ -14007,7 +14008,7 @@
       </c>
       <c r="E148" s="2">
         <f>[6]SAData!E10</f>
-        <v>1.1337100118061223</v>
+        <v>1.126120489587856</v>
       </c>
       <c r="F148" s="2">
         <f>[6]SAData!F10</f>
@@ -14049,7 +14050,7 @@
       </c>
       <c r="E149" s="2">
         <f>[6]SAData!E11</f>
-        <v>1.1607140030438332</v>
+        <v>1.1801172833283424</v>
       </c>
       <c r="F149" s="2">
         <f>[6]SAData!F11</f>
@@ -14091,7 +14092,7 @@
       </c>
       <c r="E150" s="2">
         <f>[6]SAData!E12</f>
-        <v>1.2171908200031087</v>
+        <v>1.2346824259441442</v>
       </c>
       <c r="F150" s="2">
         <f>[6]SAData!F12</f>
@@ -14133,7 +14134,7 @@
       </c>
       <c r="E151" s="2">
         <f>[6]SAData!E13</f>
-        <v>1.283558835066958</v>
+        <v>1.3075793820868926</v>
       </c>
       <c r="F151" s="2">
         <f>[6]SAData!F13</f>
@@ -14175,7 +14176,7 @@
       </c>
       <c r="E152" s="2">
         <f>[6]SAData!E14</f>
-        <v>1.4080252965623752</v>
+        <v>1.4026956155027717</v>
       </c>
       <c r="F152" s="2">
         <f>[6]SAData!F14</f>
@@ -14217,7 +14218,7 @@
       </c>
       <c r="E153" s="2">
         <f>[6]SAData!E15</f>
-        <v>1.5175964808297548</v>
+        <v>1.4979997675911214</v>
       </c>
       <c r="F153" s="2">
         <f>[6]SAData!F15</f>
@@ -14259,7 +14260,7 @@
       </c>
       <c r="E154" s="2">
         <f>[6]SAData!E16</f>
-        <v>1.5716842956517962</v>
+        <v>1.6036207419562249</v>
       </c>
       <c r="F154" s="2">
         <f>[6]SAData!F16</f>
@@ -14301,7 +14302,7 @@
       </c>
       <c r="E155" s="2">
         <f>[6]SAData!E17</f>
-        <v>1.6458238857237517</v>
+        <v>1.6532724007222435</v>
       </c>
       <c r="F155" s="2">
         <f>[6]SAData!F17</f>
@@ -14343,7 +14344,7 @@
       </c>
       <c r="E156" s="2">
         <f>[6]SAData!E18</f>
-        <v>1.717856820856833</v>
+        <v>1.7294004390193514</v>
       </c>
       <c r="F156" s="2">
         <f>[6]SAData!F18</f>
@@ -14385,7 +14386,7 @@
       </c>
       <c r="E157" s="2">
         <f>[6]SAData!E19</f>
-        <v>1.7883964032978603</v>
+        <v>1.7897568937332109</v>
       </c>
       <c r="F157" s="2">
         <f>[6]SAData!F19</f>
@@ -14427,7 +14428,7 @@
       </c>
       <c r="E158" s="2">
         <f>[6]SAData!E20</f>
-        <v>1.7941336063839641</v>
+        <v>1.8260589677338577</v>
       </c>
       <c r="F158" s="2">
         <f>[6]SAData!F20</f>
@@ -14469,7 +14470,7 @@
       </c>
       <c r="E159" s="2">
         <f>[6]SAData!E21</f>
-        <v>1.8635175216746698</v>
+        <v>1.8899834246915592</v>
       </c>
       <c r="F159" s="2">
         <f>[6]SAData!F21</f>
@@ -14511,7 +14512,7 @@
       </c>
       <c r="E160" s="2">
         <f>[6]SAData!E22</f>
-        <v>1.9065922194592113</v>
+        <v>1.976029579256867</v>
       </c>
       <c r="F160" s="2">
         <f>[6]SAData!F22</f>
@@ -14595,7 +14596,7 @@
       </c>
       <c r="E162" s="2">
         <f>[7]IRData!E3</f>
-        <v>0.9923206837799815</v>
+        <v>1.0033121086200276</v>
       </c>
       <c r="F162" s="2">
         <f>[7]IRData!F3</f>
@@ -14637,7 +14638,7 @@
       </c>
       <c r="E163" s="2">
         <f>[7]IRData!E4</f>
-        <v>1.0258154818585306</v>
+        <v>1.0189020330444378</v>
       </c>
       <c r="F163" s="2">
         <f>[7]IRData!F4</f>
@@ -14679,7 +14680,7 @@
       </c>
       <c r="E164" s="2">
         <f>[7]IRData!E5</f>
-        <v>1.0326056463787794</v>
+        <v>1.0378848863983947</v>
       </c>
       <c r="F164" s="2">
         <f>[7]IRData!F5</f>
@@ -14721,7 +14722,7 @@
       </c>
       <c r="E165" s="2">
         <f>[7]IRData!E6</f>
-        <v>1.0676674469765692</v>
+        <v>1.0625750901913893</v>
       </c>
       <c r="F165" s="2">
         <f>[7]IRData!F6</f>
@@ -14763,7 +14764,7 @@
       </c>
       <c r="E166" s="2">
         <f>[7]IRData!E7</f>
-        <v>1.0762276410999878</v>
+        <v>1.0876781311675561</v>
       </c>
       <c r="F166" s="2">
         <f>[7]IRData!F7</f>
@@ -14805,7 +14806,7 @@
       </c>
       <c r="E167" s="2">
         <f>[7]IRData!E8</f>
-        <v>1.1451203214814862</v>
+        <v>1.1320499221977611</v>
       </c>
       <c r="F167" s="2">
         <f>[7]IRData!F8</f>
@@ -14847,7 +14848,7 @@
       </c>
       <c r="E168" s="2">
         <f>[7]IRData!E9</f>
-        <v>1.2057762614790537</v>
+        <v>1.1872715086460475</v>
       </c>
       <c r="F168" s="2">
         <f>[7]IRData!F9</f>
@@ -14889,7 +14890,7 @@
       </c>
       <c r="E169" s="2">
         <f>[7]IRData!E10</f>
-        <v>1.2474506450804785</v>
+        <v>1.2494596661144923</v>
       </c>
       <c r="F169" s="2">
         <f>[7]IRData!F10</f>
@@ -14931,7 +14932,7 @@
       </c>
       <c r="E170" s="2">
         <f>[7]IRData!E11</f>
-        <v>1.3427875426021263</v>
+        <v>1.2908758337952513</v>
       </c>
       <c r="F170" s="2">
         <f>[7]IRData!F11</f>
@@ -14973,7 +14974,7 @@
       </c>
       <c r="E171" s="2">
         <f>[7]IRData!E12</f>
-        <v>1.4046771040381612</v>
+        <v>1.3750116062118418</v>
       </c>
       <c r="F171" s="2">
         <f>[7]IRData!F12</f>
@@ -15015,7 +15016,7 @@
       </c>
       <c r="E172" s="2">
         <f>[7]IRData!E13</f>
-        <v>1.4662256242124556</v>
+        <v>1.4447440859500611</v>
       </c>
       <c r="F172" s="2">
         <f>[7]IRData!F13</f>
@@ -15057,7 +15058,7 @@
       </c>
       <c r="E173" s="2">
         <f>[7]IRData!E14</f>
-        <v>1.5669527354415114</v>
+        <v>1.5333168827828205</v>
       </c>
       <c r="F173" s="2">
         <f>[7]IRData!F14</f>
@@ -15099,7 +15100,7 @@
       </c>
       <c r="E174" s="2">
         <f>[7]IRData!E15</f>
-        <v>1.7123166508885288</v>
+        <v>1.6513280651642879</v>
       </c>
       <c r="F174" s="2">
         <f>[7]IRData!F15</f>
@@ -15141,7 +15142,7 @@
       </c>
       <c r="E175" s="2">
         <f>[7]IRData!E16</f>
-        <v>1.7569037569931252</v>
+        <v>1.6936795889934797</v>
       </c>
       <c r="F175" s="2">
         <f>[7]IRData!F16</f>
@@ -15183,7 +15184,7 @@
       </c>
       <c r="E176" s="2">
         <f>[7]IRData!E17</f>
-        <v>1.7594397758824338</v>
+        <v>1.7068970430814494</v>
       </c>
       <c r="F176" s="2">
         <f>[7]IRData!F17</f>
@@ -15225,7 +15226,7 @@
       </c>
       <c r="E177" s="2">
         <f>[7]IRData!E18</f>
-        <v>1.8044561053690826</v>
+        <v>1.7243467380143345</v>
       </c>
       <c r="F177" s="2">
         <f>[7]IRData!F18</f>
@@ -15267,7 +15268,7 @@
       </c>
       <c r="E178" s="2">
         <f>[7]IRData!E19</f>
-        <v>1.7369485759342249</v>
+        <v>1.671027329007184</v>
       </c>
       <c r="F178" s="2">
         <f>[7]IRData!F19</f>
@@ -15309,7 +15310,7 @@
       </c>
       <c r="E179" s="2">
         <f>[7]IRData!E20</f>
-        <v>1.7804433072068904</v>
+        <v>1.6821511333211596</v>
       </c>
       <c r="F179" s="2">
         <f>[7]IRData!F20</f>
@@ -15351,7 +15352,7 @@
       </c>
       <c r="E180" s="2">
         <f>[7]IRData!E21</f>
-        <v>1.8469810667781668</v>
+        <v>1.6917742808198715</v>
       </c>
       <c r="F180" s="2">
         <f>[7]IRData!F21</f>
@@ -15393,7 +15394,7 @@
       </c>
       <c r="E181" s="2">
         <f>[7]IRData!E22</f>
-        <v>1.8675789761098966</v>
+        <v>1.7317523832170316</v>
       </c>
       <c r="F181" s="2">
         <f>[7]IRData!F22</f>
@@ -15477,7 +15478,7 @@
       </c>
       <c r="E183" s="2">
         <f>[8]TZData!E3</f>
-        <v>1.0210508656820274</v>
+        <v>1.0367182268975108</v>
       </c>
       <c r="F183" s="2">
         <f>[8]TZData!F3</f>
@@ -15519,7 +15520,7 @@
       </c>
       <c r="E184" s="2">
         <f>[8]TZData!E4</f>
-        <v>1.0556153313366927</v>
+        <v>1.0720661216957412</v>
       </c>
       <c r="F184" s="2">
         <f>[8]TZData!F4</f>
@@ -15561,7 +15562,7 @@
       </c>
       <c r="E185" s="2">
         <f>[8]TZData!E5</f>
-        <v>1.1099907940373888</v>
+        <v>1.1082826130812979</v>
       </c>
       <c r="F185" s="2">
         <f>[8]TZData!F5</f>
@@ -15603,7 +15604,7 @@
       </c>
       <c r="E186" s="2">
         <f>[8]TZData!E6</f>
-        <v>1.143580093612782</v>
+        <v>1.1351728279061144</v>
       </c>
       <c r="F186" s="2">
         <f>[8]TZData!F6</f>
@@ -15645,7 +15646,7 @@
       </c>
       <c r="E187" s="2">
         <f>[8]TZData!E7</f>
-        <v>1.1756384700676845</v>
+        <v>1.1640850070012463</v>
       </c>
       <c r="F187" s="2">
         <f>[8]TZData!F7</f>
@@ -15687,7 +15688,7 @@
       </c>
       <c r="E188" s="2">
         <f>[8]TZData!E8</f>
-        <v>1.206546229055788</v>
+        <v>1.2014315300214575</v>
       </c>
       <c r="F188" s="2">
         <f>[8]TZData!F8</f>
@@ -15729,7 +15730,7 @@
       </c>
       <c r="E189" s="2">
         <f>[8]TZData!E9</f>
-        <v>1.2210962860108654</v>
+        <v>1.232593595417365</v>
       </c>
       <c r="F189" s="2">
         <f>[8]TZData!F9</f>
@@ -15771,7 +15772,7 @@
       </c>
       <c r="E190" s="2">
         <f>[8]TZData!E10</f>
-        <v>1.2515828710931032</v>
+        <v>1.2654602066338621</v>
       </c>
       <c r="F190" s="2">
         <f>[8]TZData!F10</f>
@@ -15813,7 +15814,7 @@
       </c>
       <c r="E191" s="2">
         <f>[8]TZData!E11</f>
-        <v>1.2832842687413721</v>
+        <v>1.2931681655671592</v>
       </c>
       <c r="F191" s="2">
         <f>[8]TZData!F11</f>
@@ -15855,7 +15856,7 @@
       </c>
       <c r="E192" s="2">
         <f>[8]TZData!E12</f>
-        <v>1.3164204285711589</v>
+        <v>1.3280146578118128</v>
       </c>
       <c r="F192" s="2">
         <f>[8]TZData!F12</f>
@@ -15897,7 +15898,7 @@
       </c>
       <c r="E193" s="2">
         <f>[8]TZData!E13</f>
-        <v>1.3684776113712027</v>
+        <v>1.3898522836711655</v>
       </c>
       <c r="F193" s="2">
         <f>[8]TZData!F13</f>
@@ -15939,7 +15940,7 @@
       </c>
       <c r="E194" s="2">
         <f>[8]TZData!E14</f>
-        <v>1.4229926061957845</v>
+        <v>1.4327510497077038</v>
       </c>
       <c r="F194" s="2">
         <f>[8]TZData!F14</f>
@@ -15981,7 +15982,7 @@
       </c>
       <c r="E195" s="2">
         <f>[8]TZData!E15</f>
-        <v>1.4616215628210345</v>
+        <v>1.4824489763374917</v>
       </c>
       <c r="F195" s="2">
         <f>[8]TZData!F15</f>
@@ -16023,7 +16024,7 @@
       </c>
       <c r="E196" s="2">
         <f>[8]TZData!E16</f>
-        <v>1.5020071213170048</v>
+        <v>1.5324909718893391</v>
       </c>
       <c r="F196" s="2">
         <f>[8]TZData!F16</f>
@@ -16065,7 +16066,7 @@
       </c>
       <c r="E197" s="2">
         <f>[8]TZData!E17</f>
-        <v>1.5442689594453047</v>
+        <v>1.5468078837584009</v>
       </c>
       <c r="F197" s="2">
         <f>[8]TZData!F17</f>
@@ -16107,7 +16108,7 @@
       </c>
       <c r="E198" s="2">
         <f>[8]TZData!E18</f>
-        <v>1.5885418403996812</v>
+        <v>1.6281584008640875</v>
       </c>
       <c r="F198" s="2">
         <f>[8]TZData!F18</f>
@@ -16149,7 +16150,7 @@
       </c>
       <c r="E199" s="2">
         <f>[8]TZData!E19</f>
-        <v>1.6349385181151996</v>
+        <v>1.6658599441961892</v>
       </c>
       <c r="F199" s="2">
         <f>[8]TZData!F19</f>
@@ -16191,7 +16192,7 @@
       </c>
       <c r="E200" s="2">
         <f>[8]TZData!E20</f>
-        <v>1.6835627726288354</v>
+        <v>1.7130039249835767</v>
       </c>
       <c r="F200" s="2">
         <f>[8]TZData!F20</f>
@@ -16233,7 +16234,7 @@
       </c>
       <c r="E201" s="2">
         <f>[8]TZData!E21</f>
-        <v>1.7344853120686496</v>
+        <v>1.7541696811874952</v>
       </c>
       <c r="F201" s="2">
         <f>[8]TZData!F21</f>
@@ -16275,7 +16276,7 @@
       </c>
       <c r="E202" s="2">
         <f>[8]TZData!E22</f>
-        <v>1.7877585486411658</v>
+        <v>1.7970941883839631</v>
       </c>
       <c r="F202" s="2">
         <f>[8]TZData!F22</f>
@@ -16359,7 +16360,7 @@
       </c>
       <c r="E204" s="2">
         <f>[9]ZMData!E3</f>
-        <v>1.0253503606606469</v>
+        <v>1.0224901654943095</v>
       </c>
       <c r="F204" s="2">
         <f>[9]ZMData!F3</f>
@@ -16401,7 +16402,7 @@
       </c>
       <c r="E205" s="2">
         <f>[9]ZMData!E4</f>
-        <v>1.0538740327847183</v>
+        <v>1.0399701099499545</v>
       </c>
       <c r="F205" s="2">
         <f>[9]ZMData!F4</f>
@@ -16443,7 +16444,7 @@
       </c>
       <c r="E206" s="2">
         <f>[9]ZMData!E5</f>
-        <v>1.0973728039159725</v>
+        <v>1.0777929567401658</v>
       </c>
       <c r="F206" s="2">
         <f>[9]ZMData!F5</f>
@@ -16485,7 +16486,7 @@
       </c>
       <c r="E207" s="2">
         <f>[9]ZMData!E6</f>
-        <v>1.126011730223049</v>
+        <v>1.1140511839801894</v>
       </c>
       <c r="F207" s="2">
         <f>[9]ZMData!F6</f>
@@ -16527,7 +16528,7 @@
       </c>
       <c r="E208" s="2">
         <f>[9]ZMData!E7</f>
-        <v>1.2100048752017798</v>
+        <v>1.1875048984137102</v>
       </c>
       <c r="F208" s="2">
         <f>[9]ZMData!F7</f>
@@ -16569,7 +16570,7 @@
       </c>
       <c r="E209" s="2">
         <f>[9]ZMData!E8</f>
-        <v>1.2621311954601659</v>
+        <v>1.2305758921930401</v>
       </c>
       <c r="F209" s="2">
         <f>[9]ZMData!F8</f>
@@ -16611,7 +16612,7 @@
       </c>
       <c r="E210" s="2">
         <f>[9]ZMData!E9</f>
-        <v>1.3351105243839876</v>
+        <v>1.302664022117958</v>
       </c>
       <c r="F210" s="2">
         <f>[9]ZMData!F9</f>
@@ -16653,7 +16654,7 @@
       </c>
       <c r="E211" s="2">
         <f>[9]ZMData!E10</f>
-        <v>1.3520695749730507</v>
+        <v>1.3344645592351276</v>
       </c>
       <c r="F211" s="2">
         <f>[9]ZMData!F10</f>
@@ -16695,7 +16696,7 @@
       </c>
       <c r="E212" s="2">
         <f>[9]ZMData!E11</f>
-        <v>1.3869343489141379</v>
+        <v>1.355101232872514</v>
       </c>
       <c r="F212" s="2">
         <f>[9]ZMData!F11</f>
@@ -16737,7 +16738,7 @@
       </c>
       <c r="E213" s="2">
         <f>[9]ZMData!E12</f>
-        <v>1.3800954400339227</v>
+        <v>1.3517817406304078</v>
       </c>
       <c r="F213" s="2">
         <f>[9]ZMData!F12</f>
@@ -16779,7 +16780,7 @@
       </c>
       <c r="E214" s="2">
         <f>[9]ZMData!E13</f>
-        <v>1.4069868802031238</v>
+        <v>1.3907644608391989</v>
       </c>
       <c r="F214" s="2">
         <f>[9]ZMData!F13</f>
@@ -16821,7 +16822,7 @@
       </c>
       <c r="E215" s="2">
         <f>[9]ZMData!E14</f>
-        <v>1.4183370759572067</v>
+        <v>1.4033972482347783</v>
       </c>
       <c r="F215" s="2">
         <f>[9]ZMData!F14</f>
@@ -16863,7 +16864,7 @@
       </c>
       <c r="E216" s="2">
         <f>[9]ZMData!E15</f>
-        <v>1.4512935001605018</v>
+        <v>1.4318123720670304</v>
       </c>
       <c r="F216" s="2">
         <f>[9]ZMData!F15</f>
@@ -16905,7 +16906,7 @@
       </c>
       <c r="E217" s="2">
         <f>[9]ZMData!E16</f>
-        <v>1.4644390379448708</v>
+        <v>1.4564504375255525</v>
       </c>
       <c r="F217" s="2">
         <f>[9]ZMData!F16</f>
@@ -16947,7 +16948,7 @@
       </c>
       <c r="E218" s="2">
         <f>[9]ZMData!E17</f>
-        <v>1.5012008832340635</v>
+        <v>1.4949043807496252</v>
       </c>
       <c r="F218" s="2">
         <f>[9]ZMData!F17</f>
@@ -16989,7 +16990,7 @@
       </c>
       <c r="E219" s="2">
         <f>[9]ZMData!E18</f>
-        <v>1.5402035223111452</v>
+        <v>1.5320191060408039</v>
       </c>
       <c r="F219" s="2">
         <f>[9]ZMData!F18</f>
@@ -17031,7 +17032,7 @@
       </c>
       <c r="E220" s="2">
         <f>[9]ZMData!E19</f>
-        <v>1.5816270976723197</v>
+        <v>1.5725131433126012</v>
       </c>
       <c r="F220" s="2">
         <f>[9]ZMData!F19</f>
@@ -17073,7 +17074,7 @@
       </c>
       <c r="E221" s="2">
         <f>[9]ZMData!E20</f>
-        <v>1.6255938762458619</v>
+        <v>1.6215594097703909</v>
       </c>
       <c r="F221" s="2">
         <f>[9]ZMData!F20</f>
@@ -17115,7 +17116,7 @@
       </c>
       <c r="E222" s="2">
         <f>[9]ZMData!E21</f>
-        <v>1.6514862299396258</v>
+        <v>1.7196442344046197</v>
       </c>
       <c r="F222" s="2">
         <f>[9]ZMData!F21</f>
@@ -17157,7 +17158,7 @@
       </c>
       <c r="E223" s="2">
         <f>[9]ZMData!E22</f>
-        <v>1.7215693266011487</v>
+        <v>1.7738033236619906</v>
       </c>
       <c r="F223" s="2">
         <f>[9]ZMData!F22</f>

</xml_diff>